<commit_message>
update 3_python sheet Primitives
</commit_message>
<xml_diff>
--- a/data_e2setup.xlsx
+++ b/data_e2setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NGUYEN MANH DUNG\Downloads\TOOL to GEN ALL\Grok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCEB60A-0AF2-46CD-AAD4-42757060DD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5669EF7-9801-4CB3-9007-BCFB6C7916CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-3645" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primitives" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="118">
   <si>
     <t>Message_Name</t>
   </si>
@@ -373,6 +373,15 @@
   </si>
   <si>
     <t xml:space="preserve">PrintableString (SIZE(1..150, ...)) </t>
+  </si>
+  <si>
+    <t>Ext_Bit</t>
+  </si>
+  <si>
+    <t>Contain_size</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -721,22 +730,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.5703125" customWidth="1"/>
     <col min="2" max="2" width="52.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="71.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -752,8 +762,14 @@
       <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -767,8 +783,11 @@
         <v>255</v>
       </c>
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -782,8 +801,11 @@
         <v>255</v>
       </c>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -797,8 +819,11 @@
         <v>65535</v>
       </c>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -810,8 +835,11 @@
       <c r="E5" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -823,8 +851,11 @@
       <c r="E6" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="45">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45">
       <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
@@ -834,65 +865,101 @@
       <c r="E7" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>24</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="G9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>40</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1000</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>62</v>
       </c>
       <c r="B11" t="s">
         <v>63</v>
       </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
       <c r="D11">
         <v>68719476735</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>64</v>
       </c>
       <c r="B12" t="s">
         <v>63</v>
       </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
       <c r="D12">
         <v>68719476735</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>65</v>
       </c>
       <c r="B13" t="s">
         <v>66</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
       <c r="D13">
         <v>68719476735</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="30">
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -902,13 +969,25 @@
       <c r="E14" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>113</v>
       </c>
       <c r="B15" t="s">
         <v>114</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>150</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -974,7 +1053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1053,7 +1132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C8064D-1F5D-4C4A-8792-F20A50219AAE}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -1756,7 +1835,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="30">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1858,7 +1937,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" ht="30">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1883,7 +1962,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" ht="30">
+    <row r="19" spans="1:9" ht="45">
       <c r="A19" s="2" t="s">
         <v>74</v>
       </c>
@@ -2182,7 +2261,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" ht="30">
       <c r="A38" s="2" t="s">
         <v>15</v>
       </c>
@@ -2205,7 +2284,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="30">
+    <row r="39" spans="1:7" ht="45">
       <c r="A39" s="2" t="s">
         <v>74</v>
       </c>

</xml_diff>